<commit_message>
WSL2(ubuntu 22.04 LTS) on win11
</commit_message>
<xml_diff>
--- a/lj_potential_data.xlsx
+++ b/lj_potential_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inukai\Desktop\lammps_education_ch_win\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lammps_education_gcmc_win\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0FF66E-1596-497C-BD1C-2E72D415BBEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F6B7A-7474-4D46-851C-2AF409D703E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9690" yWindow="3135" windowWidth="17610" windowHeight="14490" xr2:uid="{13043327-7F88-4032-9ABE-3619D44FAB75}"/>
+    <workbookView xWindow="1275" yWindow="13530" windowWidth="16200" windowHeight="20085" xr2:uid="{13043327-7F88-4032-9ABE-3619D44FAB75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>O</t>
     <phoneticPr fontId="1"/>
@@ -144,6 +138,18 @@
   </si>
   <si>
     <t>N</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mass</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;-UFF</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -308,17 +314,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -336,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -351,19 +354,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -680,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEF2693-5B33-4C60-9C59-6324EA3992D8}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -696,315 +696,360 @@
     <col min="8" max="8" width="22.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="2">
         <v>52.84</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="2">
         <v>0.34300000000000003</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4">
+        <v>12.0107</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <f>SQRT($B$4*$F$6)</f>
         <v>39.947064973537167</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <f>($C$4+$G$6)/2</f>
         <v>0.32750000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="2">
         <v>22.14</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="2">
         <v>0.25700000000000001</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5">
+        <v>1.0079</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <f>SQRT($B$5*$F$6)</f>
         <v>25.857842137347813</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <f>($C$5+$G$6)/2</f>
         <v>0.28449999999999998</v>
       </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="18" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="2">
         <v>30.2</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="2">
         <v>0.312</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>30.2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>0.312</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="18" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="2">
         <v>38.92</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="2">
         <v>0.32629999999999998</v>
       </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="18" t="s">
+      <c r="D7">
+        <v>14.0067</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>90.58</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.36370000000000002</v>
+      </c>
+      <c r="D8">
+        <v>10.81</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B9" s="2">
         <v>10.41</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C9" s="2">
         <v>0.60199999999999998</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="18" t="s">
+      <c r="D9">
+        <v>4.0026000000000002</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B10" s="2">
         <v>141.6</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C10" s="2">
         <v>0.33500000000000002</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="18">
-        <v>104.2</v>
-      </c>
-      <c r="C10" s="18">
-        <v>0.36320000000000002</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="D10">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <f>SQRT($B$4*$F$6)*0.00008617</f>
         <v>3.4422385887696973E-3</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <f>($C$4+$G$6)/2*10</f>
         <v>3.2750000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="18">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="C11" s="18">
-        <v>0.29580000000000001</v>
-      </c>
-      <c r="E11" s="8" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>104.2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.36320000000000002</v>
+      </c>
+      <c r="D11">
+        <v>28.013999999999999</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <f>SQRT($B$5*$F$6)*0.00008617</f>
         <v>2.2281702569752608E-3</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <f>($C$5+$G$6)/2*10</f>
         <v>2.8449999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="18">
-        <v>126.3</v>
-      </c>
-      <c r="C12" s="18">
-        <v>0.3382</v>
-      </c>
-      <c r="E12" s="11" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.29580000000000001</v>
+      </c>
+      <c r="D12">
+        <v>2.016</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <f>F6*0.00008617</f>
         <v>2.602334E-3</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="16">
         <f>G6*10</f>
         <v>3.12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>126.3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.3382</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B14" s="2">
         <v>245.3</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C14" s="2">
         <v>0.37619999999999998</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="18" t="s">
+      <c r="D14">
+        <v>44.01</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B15" s="2">
         <v>161.30000000000001</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C15" s="2">
         <v>0.37209999999999999</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E16" s="8" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <f>SQRT($B$4*$F$6)*0.001987</f>
         <v>7.9374818102418351E-2</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="14">
         <f>($C$4+$G$6)/2*10</f>
         <v>3.2750000000000004</v>
       </c>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.4">
-      <c r="E17" s="8" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2">
+        <v>34.72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <f>SQRT($B$5*$F$6)*0.001987</f>
         <v>5.1379532326910109E-2</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="14">
         <f>($C$5+$G$6)/2*10</f>
         <v>2.8449999999999998</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.4">
-      <c r="E18" s="11" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="15">
         <f>F6*0.001987</f>
         <v>6.0007400000000002E-2</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="16">
         <f>G6*10</f>
         <v>3.12</v>
       </c>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="E25" t="s">
         <v>25</v>
       </c>

</xml_diff>